<commit_message>
Refactored Projectiles, Loot Drop System, Treant,
</commit_message>
<xml_diff>
--- a/TopDown_Shooter_Planning2.xlsx
+++ b/TopDown_Shooter_Planning2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity\arrow-assault\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F86E00-468F-4D3A-8DC9-76BC83138858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C314EB4B-02C2-406E-BFF2-2FECD554D258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{509F4F84-A253-417D-AE8D-5625E8E48E3B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Cooldown do tiro;</t>
   </si>
@@ -253,13 +253,31 @@
   </si>
   <si>
     <t>Implementar upgrade de sistema de coração;</t>
+  </si>
+  <si>
+    <t>Wave System Refactor</t>
+  </si>
+  <si>
+    <t>Refactor Loot System (try to make drop chances simpler)</t>
+  </si>
+  <si>
+    <t>Make enemies spread around eachother</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>Object Pooler</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +287,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -308,12 +334,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -628,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC6BEFE6-3B79-4D84-8F05-3F108B708BC2}">
-  <dimension ref="B2:H39"/>
+  <dimension ref="B2:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,12 +684,12 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4">
-        <f>SUM(B7:B39)+SUM(E7:E39)+SUM(G23:G39)</f>
-        <v>149</v>
+        <f>SUM(B7:B45)+SUM(E7:E45)+SUM(G23:G39)</f>
+        <v>156</v>
       </c>
       <c r="C4">
         <f>B4/6</f>
-        <v>24.833333333333332</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -861,7 +889,7 @@
       <c r="E17" s="3">
         <v>2</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="6" t="s">
         <v>61</v>
       </c>
       <c r="G17">
@@ -886,6 +914,12 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="3">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="G19">
         <v>2</v>
       </c>
@@ -894,12 +928,6 @@
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G20">
         <v>2</v>
       </c>
@@ -908,18 +936,6 @@
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21">
-        <v>2</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
       <c r="G21">
         <v>2</v>
       </c>
@@ -928,18 +944,6 @@
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
-        <v>2</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22" t="s">
-        <v>32</v>
-      </c>
       <c r="G22">
         <v>6</v>
       </c>
@@ -947,116 +951,77 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>3</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-      <c r="F23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25" t="s">
-        <v>53</v>
-      </c>
-    </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
-      <c r="F26" t="s">
-        <v>36</v>
+      <c r="C26" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>46</v>
+      <c r="B28" s="3">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="E28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="3">
-        <v>12</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>39</v>
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
-        <v>2</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="3">
-        <v>6</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>54</v>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1064,96 +1029,195 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="3">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>0</v>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="E32">
         <v>2</v>
       </c>
       <c r="F32" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="3">
-        <v>4</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>69</v>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
       </c>
       <c r="E33">
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>45</v>
+      </c>
+      <c r="E35" s="3">
+        <v>12</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>2</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E36" s="3">
+        <v>6</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
         <v>1</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C38" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>4</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="3">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E34">
-        <v>2</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E35">
-        <v>2</v>
-      </c>
-      <c r="F35" t="s">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="F36" t="s">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37" t="s">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E38">
-        <v>2</v>
-      </c>
-      <c r="F38" t="s">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E39">
-        <v>2</v>
-      </c>
-      <c r="F39" t="s">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
         <v>52</v>
       </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>